<commit_message>
Grindbridge adjust + BOM + hardware inclusion beggining
</commit_message>
<xml_diff>
--- a/BOM/DeckandMold/DeckMoldBOM.xlsx
+++ b/BOM/DeckandMold/DeckMoldBOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="73">
   <si>
     <t>Item Name</t>
   </si>
@@ -216,6 +216,33 @@
   </si>
   <si>
     <t>72"*40" 3/32Thickness</t>
+  </si>
+  <si>
+    <t>Mold</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t>*** squeegy</t>
+  </si>
+  <si>
+    <t>**buckets</t>
+  </si>
+  <si>
+    <t>Cleaning Material</t>
+  </si>
+  <si>
+    <t>https://www.fiberglasshawaii.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*** saftey </t>
+  </si>
+  <si>
+    <t>gloves</t>
+  </si>
+  <si>
+    <t>breathing mask</t>
   </si>
 </sst>
 </file>
@@ -582,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00748F7B-54B9-4908-9896-05F30F59DACC}">
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,7 +626,7 @@
     <col min="13" max="13" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -637,10 +664,13 @@
         <v>42</v>
       </c>
       <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -677,7 +707,7 @@
         <v>75.546000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -714,7 +744,7 @@
         <v>356.346</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -747,7 +777,7 @@
         <v>113.346</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>27</v>
       </c>
@@ -783,7 +813,7 @@
         <v>48.546000000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -819,7 +849,7 @@
         <v>11.826000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -856,7 +886,7 @@
         <v>21.545999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -893,7 +923,7 @@
         <v>43.146000000000008</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>37</v>
       </c>
@@ -930,7 +960,7 @@
         <v>18.306000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>31</v>
       </c>
@@ -966,7 +996,7 @@
         <v>29.106000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -1002,7 +1032,7 @@
         <v>58.298400000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -1032,7 +1062,7 @@
         <v>7.5384000000000011</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>46</v>
       </c>
@@ -1068,7 +1098,7 @@
         <v>69.638400000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>52</v>
       </c>
@@ -1108,7 +1138,7 @@
         <v>869.33520000000021</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>56</v>
       </c>
@@ -1145,12 +1175,12 @@
         <v>264.54599999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1187,11 +1217,11 @@
       <c r="L21" t="s">
         <v>42</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>5</v>
@@ -1228,7 +1258,7 @@
         <v>75.546000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>56</v>
       </c>
@@ -1265,7 +1295,7 @@
         <v>264.54599999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>24</v>
       </c>
@@ -1294,11 +1324,11 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L23:L34" si="3">E24*F24*I24*(1+J24)</f>
+        <f t="shared" ref="L24:L34" si="3">E24*F24*I24*(1+J24)</f>
         <v>113.346</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>27</v>
       </c>
@@ -1333,329 +1363,903 @@
         <f t="shared" si="3"/>
         <v>48.546000000000006</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="M25">
+        <f>SUM(L22:L25)</f>
+        <v>501.98399999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E26">
+      <c r="E27">
         <v>10.95</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
         <v>35</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H27" t="s">
         <v>36</v>
       </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>0.08</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="3"/>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0.08</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>E27*F27*I27*(1+J27)</f>
         <v>11.826000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E27">
+      <c r="E28">
         <f>19.95/5</f>
         <v>3.9899999999999998</v>
       </c>
-      <c r="F27">
+      <c r="F28">
         <v>5</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" t="s">
         <v>11</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>39</v>
       </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>0.08</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="3"/>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>0.08</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>E28*F28*I28*(1+J28)</f>
         <v>21.545999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>19</v>
       </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E28">
+      <c r="E29">
         <f>39.95/3</f>
         <v>13.316666666666668</v>
       </c>
-      <c r="F28">
+      <c r="F29">
         <v>3</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>11</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H29" t="s">
         <v>38</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>0.08</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="3"/>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0.08</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f>E29*F29*I29*(1+J29)</f>
         <v>43.146000000000008</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>37</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E29">
+      <c r="E30">
         <f>16.95/3</f>
         <v>5.6499999999999995</v>
       </c>
-      <c r="F29">
+      <c r="F30">
         <v>3</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" t="s">
         <v>11</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H30" t="s">
         <v>38</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>0.08</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="3"/>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>0.08</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f>E30*F30*I30*(1+J30)</f>
         <v>18.306000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E30">
+      <c r="E31">
         <v>26.95</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
         <v>32</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H31" t="s">
         <v>33</v>
       </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>0.08</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="3"/>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0.08</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f>E31*F31*I31*(1+J31)</f>
         <v>29.106000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32">
+        <v>14.95</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>53</v>
+      </c>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>0.08</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>E32*F32*I32*(1+J32)</f>
+        <v>16.146000000000001</v>
+      </c>
+      <c r="M32">
+        <f>SUM(L27:L32)</f>
+        <v>140.07600000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>12</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C35" t="s">
         <v>13</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D35" t="s">
         <v>14</v>
       </c>
-      <c r="E31">
+      <c r="E35">
         <v>26.99</v>
       </c>
-      <c r="F31">
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G35" t="s">
         <v>44</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H35" t="s">
         <v>17</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
-        <v>0.08</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="3"/>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>0.08</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f>E35*F35*I35*(1+J35)</f>
         <v>58.298400000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D36" t="s">
         <v>14</v>
       </c>
-      <c r="E32">
+      <c r="E36">
         <v>6.98</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>0.08</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="3"/>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>0.08</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>E36*F36*I36*(1+J36)</f>
         <v>7.5384000000000011</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>61</v>
       </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E33">
+      <c r="E37">
         <v>40.74</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="s">
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
         <v>44</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H37" t="s">
         <v>63</v>
       </c>
-      <c r="I33">
-        <v>1</v>
-      </c>
-      <c r="J33">
-        <v>0.08</v>
-      </c>
-      <c r="K33">
-        <v>0</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="3"/>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>0.08</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f>E37*F37*I37*(1+J37)</f>
         <v>43.999200000000002</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
+      <c r="M37">
+        <f>SUM(L35:L37)</f>
+        <v>109.836</v>
+      </c>
+      <c r="N37">
+        <f>SUM(M22:M37)</f>
+        <v>751.89599999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L39" t="s">
+        <v>70</v>
+      </c>
+      <c r="M39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L40" t="s">
+        <v>66</v>
+      </c>
+      <c r="M40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L43" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1</v>
+      </c>
+      <c r="D45" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F45" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="H45" t="s">
+        <v>16</v>
+      </c>
+      <c r="I45" t="s">
+        <v>47</v>
+      </c>
+      <c r="J45" t="s">
+        <v>48</v>
+      </c>
+      <c r="K45" t="s">
+        <v>49</v>
+      </c>
+      <c r="L45" t="s">
+        <v>42</v>
+      </c>
+      <c r="N45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E46">
+        <v>69.95</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>0.08</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f>E46*F46*I46*(1+J46)</f>
+        <v>75.546000000000006</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47">
+        <f>244.95/3</f>
+        <v>81.649999999999991</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>57</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>0.08</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ref="L47:L49" si="4">E47*F47*I47*(1+J47)</f>
+        <v>264.54599999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48">
+        <v>104.95</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>0.08</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="4"/>
+        <v>113.346</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49">
+        <v>44.95</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0.08</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <f t="shared" si="4"/>
+        <v>48.546000000000006</v>
+      </c>
+      <c r="M49">
+        <f>SUM(L46:L49)</f>
+        <v>501.98399999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E51">
+        <v>10.95</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>35</v>
+      </c>
+      <c r="H51" t="s">
+        <v>36</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0.08</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <f>E51*F51*I51*(1+J51)</f>
+        <v>11.826000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <f>19.95/5</f>
+        <v>3.9899999999999998</v>
+      </c>
+      <c r="F52">
+        <v>5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>39</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>0.08</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <f>E52*F52*I52*(1+J52)</f>
+        <v>21.545999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E53">
+        <f>39.95/3</f>
+        <v>13.316666666666668</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>38</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>0.08</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <f>E53*F53*I53*(1+J53)</f>
+        <v>43.146000000000008</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E54">
+        <f>16.95/3</f>
+        <v>5.6499999999999995</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>38</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>0.08</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <f>E54*F54*I54*(1+J54)</f>
+        <v>18.306000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E55">
+        <v>26.95</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55" t="s">
+        <v>32</v>
+      </c>
+      <c r="H55" t="s">
+        <v>33</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>0.08</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <f>E55*F55*I55*(1+J55)</f>
+        <v>29.106000000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>52</v>
       </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E34">
+      <c r="E56">
         <v>14.95</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
         <v>53</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H56" t="s">
         <v>54</v>
       </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="J34">
-        <v>0.08</v>
-      </c>
-      <c r="K34">
-        <v>0</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="3"/>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>0.08</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <f>E56*F56*I56*(1+J56)</f>
         <v>16.146000000000001</v>
       </c>
-      <c r="M34">
-        <f>SUM(L22:L34)</f>
+      <c r="M56">
+        <f>SUM(L51:L56)</f>
+        <v>140.07600000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" t="s">
+        <v>13</v>
+      </c>
+      <c r="D59" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59">
+        <v>26.99</v>
+      </c>
+      <c r="F59">
+        <v>2</v>
+      </c>
+      <c r="G59" t="s">
+        <v>44</v>
+      </c>
+      <c r="H59" t="s">
+        <v>17</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>0.08</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <f>E59*F59*I59*(1+J59)</f>
+        <v>58.298400000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
+        <v>13</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60">
+        <v>6.98</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0.08</v>
+      </c>
+      <c r="K60">
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <f>E60*F60*I60*(1+J60)</f>
+        <v>7.5384000000000011</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>61</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E61">
+        <v>40.74</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
+        <v>44</v>
+      </c>
+      <c r="H61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>0.08</v>
+      </c>
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <f>E61*F61*I61*(1+J61)</f>
+        <v>43.999200000000002</v>
+      </c>
+      <c r="M61">
+        <f>SUM(L59:L61)</f>
+        <v>109.836</v>
+      </c>
+      <c r="N61">
+        <f>SUM(M46:M61)</f>
         <v>751.89599999999996</v>
       </c>
     </row>
@@ -1663,9 +2267,12 @@
   <hyperlinks>
     <hyperlink ref="D16" r:id="rId1" xr:uid="{77AC9A19-5473-4229-92A0-56E2ABA515DF}"/>
     <hyperlink ref="D23" r:id="rId2" xr:uid="{206FC96B-D99D-4EF8-8A72-1028E2C35148}"/>
-    <hyperlink ref="D33" r:id="rId3" location="8734k24/=1997idd" xr:uid="{DDBB5CA6-7F38-4CF4-9778-18CDAC77C9C8}"/>
+    <hyperlink ref="D37" r:id="rId3" location="8734k24/=1997idd" xr:uid="{DDBB5CA6-7F38-4CF4-9778-18CDAC77C9C8}"/>
+    <hyperlink ref="L43" r:id="rId4" xr:uid="{ABD62DFF-2716-4781-B17D-55E242AF5EB4}"/>
+    <hyperlink ref="D47" r:id="rId5" xr:uid="{2D8BBBD3-C811-4CC2-A9D8-4DA0B379FA7F}"/>
+    <hyperlink ref="D61" r:id="rId6" location="8734k24/=1997idd" xr:uid="{3691220A-09DD-45CD-9976-735E94AD247C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
battery spacer and contact re-designed
</commit_message>
<xml_diff>
--- a/BOM/DeckandMold/DeckMoldBOM.xlsx
+++ b/BOM/DeckandMold/DeckMoldBOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\LongboardMarkII\BOM\DeckandMold\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MarkII\LongboardMarkII\BOM\DeckandMold\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -309,7 +309,22 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,10 +362,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -674,901 +690,905 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" customWidth="1"/>
-    <col min="10" max="10" width="5" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="11.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>26.99</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0.08</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <f>E2*F2*I2*(1+J2)</f>
+      <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <f t="shared" ref="L2:L7" si="0">E2*F2*I2*(1+J2)</f>
         <v>58.298400000000001</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <f>L2+K2</f>
         <v>58.298400000000001</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <f>IF(C2="Y",0,N2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>6.98</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.08</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <f>E3*F3*I3*(1+J3)</f>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <f t="shared" si="0"/>
         <v>7.5384000000000011</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <f>L3+K3+N2</f>
         <v>65.836799999999997</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <f>IF(C3="Y",O2,K3+L3+O2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>34.99</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0.08</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <f>E4*F4*I4*(1+J4)</f>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <f t="shared" si="0"/>
         <v>37.789200000000008</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4" si="0">L4+K4+N3</f>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4" si="1">L4+K4+N3</f>
         <v>103.626</v>
       </c>
-      <c r="O4">
-        <f t="shared" ref="O4" si="1">IF(C4="Y",O3,K4+L4+O3)</f>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4" si="2">IF(C4="Y",O3,K4+L4+O3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>10</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.08</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <f>E5*F5*I5*(1+J5)</f>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="0"/>
         <v>10.8</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <f>L5+K5+N4</f>
         <v>114.426</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <f>IF(C5="Y",O4,K5+L5+O4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>20</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <f>E6*F6*I6*(1+J6)</f>
+      <c r="I6" s="1">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <f>L6+K6+N5</f>
         <v>174.42599999999999</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <f>IF(C6="Y",O5,K6+L6+O5)</f>
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>218.14</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>0.08</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <f>E7*F7*I7*(1+J7)</f>
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="0"/>
         <v>235.59120000000001</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <f>L7+K7+N6</f>
         <v>410.0172</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N10" t="s">
+      <c r="N10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O10" t="s">
+      <c r="O10" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>10.95</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>0.08</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <f t="shared" ref="L11:L16" si="2">E11*F11*I11*(1+J11)</f>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" ref="L11:L16" si="3">E11*F11*I11*(1+J11)</f>
         <v>11.826000000000001</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <f>L11+K11</f>
         <v>11.826000000000001</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <f>IF(C11="Y",0,K11+L11)</f>
         <v>11.826000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <f>19.95/5</f>
         <v>3.9899999999999998</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>5</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>0.08</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
         <v>21.545999999999999</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <f>L12+K12+N11</f>
         <v>33.372</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <f>IF(C12="Y",O11,K12+L12+O11)</f>
         <v>33.372</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <f>39.95/3</f>
         <v>13.316666666666668</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>0.08</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="2"/>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1">
+        <f t="shared" si="3"/>
         <v>43.146000000000008</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="1">
         <f>L13+K13+N12</f>
         <v>76.518000000000001</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <f>IF(C13="Y",O12,K13+L13+O12)</f>
         <v>76.518000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <f>16.95/3</f>
         <v>5.6499999999999995</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="1">
         <v>3</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0.08</v>
-      </c>
-      <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="2"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <f t="shared" si="3"/>
         <v>18.306000000000001</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="1">
         <f>L14+K14+N13</f>
         <v>94.823999999999998</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <f>IF(C14="Y",O13,K14+L14+O13)</f>
         <v>94.823999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>26.95</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>0.08</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="2"/>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="3"/>
         <v>29.106000000000002</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="1">
         <f>L15+K15+N14</f>
         <v>123.93</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <f>IF(C15="Y",O14,K15+L15+O14)</f>
         <v>123.93</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>14.95</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>0.08</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="2"/>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" si="3"/>
         <v>16.146000000000001</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="1">
         <f>L16+K16+N15</f>
         <v>140.07600000000002</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="1">
         <f>IF(C16="Y",O15,K16+L16+O15)</f>
         <v>140.07600000000002</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B19" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K19" t="s">
+      <c r="K19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N19" t="s">
+      <c r="N19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O19" t="s">
+      <c r="O19" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>69.95</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>0.08</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
         <f>E20*F20*I20*(1+J20)</f>
         <v>75.546000000000006</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="1">
         <f>L20+K20</f>
         <v>75.546000000000006</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="1">
         <f>IF(C20="Y",0,N20)</f>
         <v>75.546000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <f>329.95/5</f>
         <v>65.989999999999995</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>5</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>0.08</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21">
-        <f t="shared" ref="L21:L23" si="3">E21*F21*I21*(1+J21)</f>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <f t="shared" ref="L21:L23" si="4">E21*F21*I21*(1+J21)</f>
         <v>356.346</v>
       </c>
-      <c r="N21">
-        <f t="shared" ref="N21:N24" si="4">L21+K21</f>
+      <c r="N21" s="1">
+        <f t="shared" ref="N21:N24" si="5">L21+K21</f>
         <v>356.346</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="1">
         <f>IF(C21="Y",O20,K21+L21+O20)</f>
         <v>431.892</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>104.95</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0.08</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="3"/>
-        <v>113.346</v>
-      </c>
-      <c r="N22">
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
         <f t="shared" si="4"/>
         <v>113.346</v>
       </c>
-      <c r="O22">
-        <f t="shared" ref="O22:O23" si="5">IF(C22="Y",O21,K22+L22+O21)</f>
+      <c r="N22" s="1">
+        <f t="shared" si="5"/>
+        <v>113.346</v>
+      </c>
+      <c r="O22" s="1">
+        <f t="shared" ref="O22:O23" si="6">IF(C22="Y",O21,K22+L22+O21)</f>
         <v>545.23800000000006</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>44.95</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>0.08</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="3"/>
-        <v>48.546000000000006</v>
-      </c>
-      <c r="N23">
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
         <f t="shared" si="4"/>
         <v>48.546000000000006</v>
       </c>
-      <c r="O23">
+      <c r="N23" s="1">
         <f t="shared" si="5"/>
+        <v>48.546000000000006</v>
+      </c>
+      <c r="O23" s="1">
+        <f t="shared" si="6"/>
         <v>593.78400000000011</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>64.48</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>0.08</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
         <f>E24*F24*I24*(1+J24)</f>
         <v>69.638400000000004</v>
       </c>
-      <c r="N24">
-        <f t="shared" si="4"/>
+      <c r="N24" s="1">
+        <f t="shared" si="5"/>
         <v>69.638400000000004</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="1">
         <f>IF(C24="Y",O23,K24+L24+O23)</f>
         <v>663.42240000000015</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="1">
         <f>SUM(O24,O16,O5)</f>
         <v>803.49840000000017</v>
       </c>
@@ -1580,528 +1600,528 @@
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B27" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>69.95</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-      <c r="J28">
-        <v>0.08</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
         <f>E28*F28*I28*(1+J28)</f>
         <v>75.546000000000006</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="1">
         <f>L28+K28</f>
         <v>75.546000000000006</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="1">
         <f>IF(C28="Y",0,N28)</f>
         <v>75.546000000000006</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <f>244.95/3</f>
         <v>81.649999999999991</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-      <c r="J29">
-        <v>0.08</v>
-      </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29">
-        <f t="shared" ref="L29" si="6">E29*F29*I29*(1+J29)</f>
+      <c r="I29" s="1">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" ref="L29" si="7">E29*F29*I29*(1+J29)</f>
         <v>264.54599999999999</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="1">
         <f>L29+K29+N28</f>
         <v>340.09199999999998</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="1">
         <f>IF(C29="Y",O28,K29+L29+O28)</f>
         <v>340.09199999999998</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>104.95</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="F30" s="1">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-      <c r="J30">
-        <v>0.08</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <f t="shared" ref="L30:L31" si="7">E30*F30*I30*(1+J30)</f>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" ref="L30:L31" si="8">E30*F30*I30*(1+J30)</f>
         <v>113.346</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="1">
         <f>L30+K30+N29</f>
         <v>453.43799999999999</v>
       </c>
-      <c r="O30">
-        <f t="shared" ref="O30:O31" si="8">IF(C30="Y",O29,K30+L30+O29)</f>
+      <c r="O30" s="1">
+        <f t="shared" ref="O30:O31" si="9">IF(C30="Y",O29,K30+L30+O29)</f>
         <v>453.43799999999999</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
+      <c r="B31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>44.95</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
-        <v>0.08</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="7"/>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="8"/>
         <v>48.546000000000006</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="1">
         <f>L31+K31+N30</f>
         <v>501.98399999999998</v>
       </c>
-      <c r="O31">
-        <f t="shared" si="8"/>
+      <c r="O31" s="1">
+        <f t="shared" si="9"/>
         <v>501.98399999999998</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>40.74</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="F32" s="1">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I32">
-        <v>1</v>
-      </c>
-      <c r="J32">
-        <v>0.08</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
+      <c r="I32" s="1">
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1">
         <f>E32*F32*I32*(1+J32)</f>
         <v>43.999200000000002</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="1">
         <f>L32+K32+N15</f>
         <v>167.92920000000001</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="1">
         <f>IF(C32="Y",O31,K32+L32+O31)</f>
         <v>545.98320000000001</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="1">
         <f>SUM(O32,O16,O5)</f>
         <v>686.05920000000003</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B34" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G34" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K34" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M34" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O34" t="s">
+      <c r="O34" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+      <c r="B36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <f>60.45/5</f>
         <v>12.09</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="1">
         <v>5</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-      <c r="J36">
-        <v>0.08</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <f t="shared" ref="L36:L38" si="9">E36*F36*I36*(1+J36)</f>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0</v>
+      </c>
+      <c r="L36" s="1">
+        <f t="shared" ref="L36:L38" si="10">E36*F36*I36*(1+J36)</f>
         <v>65.286000000000001</v>
       </c>
-      <c r="N36">
-        <f t="shared" ref="N36:N38" si="10">L36+K36</f>
+      <c r="N36" s="1">
+        <f t="shared" ref="N36:N38" si="11">L36+K36</f>
         <v>65.286000000000001</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="1">
         <f>IF(C36="Y",O35,K36+L36+O35)</f>
         <v>65.286000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
+      <c r="B37" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>104.95</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="s">
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="J37">
-        <v>0.08</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <f t="shared" si="9"/>
-        <v>113.346</v>
-      </c>
-      <c r="N37">
+      <c r="I37" s="1">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0</v>
+      </c>
+      <c r="L37" s="1">
         <f t="shared" si="10"/>
         <v>113.346</v>
       </c>
-      <c r="O37">
-        <f t="shared" ref="O37:O38" si="11">IF(C37="Y",O36,K37+L37+O36)</f>
+      <c r="N37" s="1">
+        <f t="shared" si="11"/>
+        <v>113.346</v>
+      </c>
+      <c r="O37" s="1">
+        <f t="shared" ref="O37:O38" si="12">IF(C37="Y",O36,K37+L37+O36)</f>
         <v>178.63200000000001</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
+      <c r="B38" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>44.95</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38" t="s">
+      <c r="F38" s="1">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H38" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="J38">
-        <v>0.08</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="9"/>
-        <v>48.546000000000006</v>
-      </c>
-      <c r="N38">
+      <c r="I38" s="1">
+        <v>1</v>
+      </c>
+      <c r="J38" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="1">
         <f t="shared" si="10"/>
         <v>48.546000000000006</v>
       </c>
-      <c r="O38">
+      <c r="N38" s="1">
         <f t="shared" si="11"/>
+        <v>48.546000000000006</v>
+      </c>
+      <c r="O38" s="1">
+        <f t="shared" si="12"/>
         <v>227.178</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>64.48</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I39">
-        <v>1</v>
-      </c>
-      <c r="J39">
-        <v>0.08</v>
-      </c>
-      <c r="K39">
-        <v>0</v>
-      </c>
-      <c r="L39">
+      <c r="I39" s="1">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+      <c r="L39" s="1">
         <f>E39*F39*I39*(1+J39)</f>
         <v>69.638400000000004</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="1">
         <f>L39+K39</f>
         <v>69.638400000000004</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="1">
         <f>IF(C39="Y",O38,K39+L39+O38)</f>
         <v>296.81639999999999</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="1">
         <f>SUM(O39,O16,O5)</f>
         <v>436.89240000000001</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L55" t="s">
+      <c r="L55" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L56" t="s">
+      <c r="L56" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M56" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L57" t="s">
+      <c r="L57" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="L58" t="s">
+      <c r="L58" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2111,496 +2131,496 @@
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C61" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="B61" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G61" t="s">
+      <c r="G61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H61" t="s">
+      <c r="H61" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I61" t="s">
+      <c r="I61" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J61" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K61" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L61" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N61" t="s">
+      <c r="N61" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O61" t="s">
+      <c r="O61" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="1">
         <f>60.45/5</f>
         <v>12.09</v>
       </c>
-      <c r="F63">
+      <c r="F63" s="1">
         <v>5</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-      <c r="J63">
-        <v>0.08</v>
-      </c>
-      <c r="K63">
-        <v>0</v>
-      </c>
-      <c r="L63">
-        <f t="shared" ref="L63:L65" si="12">E63*F63*I63*(1+J63)</f>
+      <c r="I63" s="1">
+        <v>1</v>
+      </c>
+      <c r="J63" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K63" s="1">
+        <v>0</v>
+      </c>
+      <c r="L63" s="1">
+        <f t="shared" ref="L63:L65" si="13">E63*F63*I63*(1+J63)</f>
         <v>65.286000000000001</v>
       </c>
-      <c r="N63">
+      <c r="N63" s="1">
         <f>L63+K63+N62</f>
         <v>65.286000000000001</v>
       </c>
-      <c r="O63">
+      <c r="O63" s="1">
         <f>IF(C63="Y",O62,K63+L63+O62)</f>
         <v>65.286000000000001</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B64" t="s">
+      <c r="B64" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="1">
         <v>104.95</v>
       </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64" t="s">
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I64">
-        <v>1</v>
-      </c>
-      <c r="J64">
-        <v>0.08</v>
-      </c>
-      <c r="K64">
-        <v>0</v>
-      </c>
-      <c r="L64">
-        <f t="shared" si="12"/>
+      <c r="I64" s="1">
+        <v>1</v>
+      </c>
+      <c r="J64" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <f t="shared" si="13"/>
         <v>113.346</v>
       </c>
-      <c r="N64">
+      <c r="N64" s="1">
         <f>L64+K64+N63</f>
         <v>178.63200000000001</v>
       </c>
-      <c r="O64">
+      <c r="O64" s="1">
         <f>IF(C64="Y",O63,K64+L64+O63)</f>
         <v>178.63200000000001</v>
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B65" t="s">
+      <c r="B65" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="1">
         <v>44.95</v>
       </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="F65" s="1">
+        <v>1</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H65" t="s">
+      <c r="H65" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I65">
-        <v>1</v>
-      </c>
-      <c r="J65">
-        <v>0.08</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <f t="shared" si="12"/>
+      <c r="I65" s="1">
+        <v>1</v>
+      </c>
+      <c r="J65" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K65" s="1">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1">
+        <f t="shared" si="13"/>
         <v>48.546000000000006</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="1">
         <f>SUM(L62:L65)</f>
         <v>227.178</v>
       </c>
-      <c r="N65">
+      <c r="N65" s="1">
         <f>L65+K65+N64</f>
         <v>227.178</v>
       </c>
-      <c r="O65">
+      <c r="O65" s="1">
         <f>IF(C65="Y",O64,K65+L65+O64)</f>
         <v>227.178</v>
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="1">
         <v>40.74</v>
       </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66" t="s">
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H66" t="s">
+      <c r="H66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="I66">
-        <v>1</v>
-      </c>
-      <c r="J66">
-        <v>0.08</v>
-      </c>
-      <c r="K66">
-        <v>0</v>
-      </c>
-      <c r="L66">
+      <c r="I66" s="1">
+        <v>1</v>
+      </c>
+      <c r="J66" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K66" s="1">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1">
         <f>E66*F66*I66*(1+J66)</f>
         <v>43.999200000000002</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="1">
         <f>SUM(L65:L72)</f>
         <v>232.62120000000004</v>
       </c>
-      <c r="N66" t="e">
+      <c r="N66" s="1" t="e">
         <f>L66+K66+N72</f>
         <v>#REF!</v>
       </c>
-      <c r="O66" t="e">
+      <c r="O66" s="1" t="e">
         <f>IF(C66="Y",O72,K66+L66+O72)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+      <c r="B67" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="1">
         <v>10.95</v>
       </c>
-      <c r="F67">
-        <v>1</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I67">
-        <v>1</v>
-      </c>
-      <c r="J67">
-        <v>0.08</v>
-      </c>
-      <c r="K67">
-        <v>0</v>
-      </c>
-      <c r="L67">
-        <f t="shared" ref="L67:L72" si="13">E67*F67*I67*(1+J67)</f>
+      <c r="I67" s="1">
+        <v>1</v>
+      </c>
+      <c r="J67" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <f t="shared" ref="L67:L72" si="14">E67*F67*I67*(1+J67)</f>
         <v>11.826000000000001</v>
       </c>
-      <c r="N67" t="e">
+      <c r="N67" s="1" t="e">
         <f>L67+K67+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="O67" t="e">
+      <c r="O67" s="1" t="e">
         <f>IF(C67="Y",#REF!,K67+L67+#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
+      <c r="B68" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="1">
         <f>19.95/5</f>
         <v>3.9899999999999998</v>
       </c>
-      <c r="F68">
+      <c r="F68" s="1">
         <v>5</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H68" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I68">
-        <v>1</v>
-      </c>
-      <c r="J68">
-        <v>0.08</v>
-      </c>
-      <c r="K68">
-        <v>0</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="13"/>
+      <c r="I68" s="1">
+        <v>1</v>
+      </c>
+      <c r="J68" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K68" s="1">
+        <v>0</v>
+      </c>
+      <c r="L68" s="1">
+        <f t="shared" si="14"/>
         <v>21.545999999999999</v>
       </c>
-      <c r="N68" t="e">
+      <c r="N68" s="1" t="e">
         <f>L68+K68+N67</f>
         <v>#REF!</v>
       </c>
-      <c r="O68" t="e">
+      <c r="O68" s="1" t="e">
         <f>IF(C68="Y",O67,K68+L68+O67)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="B69" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="1">
         <f>39.95/3</f>
         <v>13.316666666666668</v>
       </c>
-      <c r="F69">
+      <c r="F69" s="1">
         <v>3</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H69" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I69">
-        <v>1</v>
-      </c>
-      <c r="J69">
-        <v>0.08</v>
-      </c>
-      <c r="K69">
-        <v>0</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="13"/>
+      <c r="I69" s="1">
+        <v>1</v>
+      </c>
+      <c r="J69" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K69" s="1">
+        <v>0</v>
+      </c>
+      <c r="L69" s="1">
+        <f t="shared" si="14"/>
         <v>43.146000000000008</v>
       </c>
-      <c r="N69" t="e">
+      <c r="N69" s="1" t="e">
         <f>L69+K69+N68</f>
         <v>#REF!</v>
       </c>
-      <c r="O69" t="e">
+      <c r="O69" s="1" t="e">
         <f>IF(C69="Y",O68,K69+L69+O68)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="1">
         <f>16.95/3</f>
         <v>5.6499999999999995</v>
       </c>
-      <c r="F70">
+      <c r="F70" s="1">
         <v>3</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H70" t="s">
+      <c r="H70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I70">
-        <v>1</v>
-      </c>
-      <c r="J70">
-        <v>0.08</v>
-      </c>
-      <c r="K70">
-        <v>0</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="13"/>
+      <c r="I70" s="1">
+        <v>1</v>
+      </c>
+      <c r="J70" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K70" s="1">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1">
+        <f t="shared" si="14"/>
         <v>18.306000000000001</v>
       </c>
-      <c r="N70" t="e">
+      <c r="N70" s="1" t="e">
         <f>L70+K70+N69</f>
         <v>#REF!</v>
       </c>
-      <c r="O70" t="e">
+      <c r="O70" s="1" t="e">
         <f>IF(C70="Y",O69,K70+L70+O69)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="B71" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="1">
         <v>26.95</v>
       </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-      <c r="G71" t="s">
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H71" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I71">
-        <v>1</v>
-      </c>
-      <c r="J71">
-        <v>0.08</v>
-      </c>
-      <c r="K71">
-        <v>0</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="13"/>
+      <c r="I71" s="1">
+        <v>1</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1">
+        <f t="shared" si="14"/>
         <v>29.106000000000002</v>
       </c>
-      <c r="N71" t="e">
+      <c r="N71" s="1" t="e">
         <f>L71+K71+N70</f>
         <v>#REF!</v>
       </c>
-      <c r="O71" t="e">
+      <c r="O71" s="1" t="e">
         <f>IF(C71="Y",O70,K71+L71+O70)</f>
         <v>#REF!</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+      <c r="B72" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="1">
         <v>14.95</v>
       </c>
-      <c r="F72">
-        <v>1</v>
-      </c>
-      <c r="G72" t="s">
+      <c r="F72" s="1">
+        <v>1</v>
+      </c>
+      <c r="G72" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H72" t="s">
+      <c r="H72" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I72">
-        <v>1</v>
-      </c>
-      <c r="J72">
-        <v>0.08</v>
-      </c>
-      <c r="K72">
-        <v>0</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="13"/>
+      <c r="I72" s="1">
+        <v>1</v>
+      </c>
+      <c r="J72" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="K72" s="1">
+        <v>0</v>
+      </c>
+      <c r="L72" s="1">
+        <f t="shared" si="14"/>
         <v>16.146000000000001</v>
       </c>
-      <c r="N72" t="e">
+      <c r="N72" s="1" t="e">
         <f>L72+K72+N71</f>
         <v>#REF!</v>
       </c>
-      <c r="O72" t="e">
+      <c r="O72" s="1" t="e">
         <f>IF(C72="Y",O71,K72+L72+O71)</f>
         <v>#REF!</v>
       </c>

</xml_diff>